<commit_message>
Feature/1687 wrap up sumo model v3 (#247)
# PR Context
- Changes to address findings in wrap up of Sumo model 3 update.
---------

Signed-off-by: erichesse <hessee@rki.de>
Signed-off-by: Janina Esins <esinsj@rki.de>
Co-authored-by: erichesse <hessee@rki.de>
Co-authored-by: rababerladuseladim <rababerladuseladim@users.noreply.github.com>
Co-authored-by: esinsj <72222648+esinsj@users.noreply.github.com>
Co-authored-by: Nicolas Drebenstedt <897972+cutoffthetop@users.noreply.github.com>
Co-authored-by: RKI | Metadata Exchange <121876825+RKIMetadataExchange@users.noreply.github.com>
Co-authored-by: RKIMetadataExchange <mex@rki.de>
</commit_message>
<xml_diff>
--- a/assets/raw-data/sumo/cc2_aux_valuesets_v3.0.3.xlsx
+++ b/assets/raw-data/sumo/cc2_aux_valuesets_v3.0.3.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HesseE\mex-extractors\assets\raw-data\sumo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alik\Documents\workspace\mex-extractors\assets\raw-data\sumo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CD8A5B-E30D-4E50-B0A0-4A8BCA9125E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9E253A-90B7-47C4-A475-148F1719AD87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="aux_cedis_groups" sheetId="1" r:id="rId1"/>
+    <sheet name="aux_cedis_group" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">aux_cedis_groups!$A$1:$C$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">aux_cedis_group!$A$1:$C$21</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -179,7 +179,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -486,7 +486,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="48.85546875" style="4" bestFit="1" customWidth="1"/>

</xml_diff>